<commit_message>
First batch of files
</commit_message>
<xml_diff>
--- a/000 Dokumenty Ogolne/04 Oferty dla klientow/001 Spis ofert.xlsx
+++ b/000 Dokumenty Ogolne/04 Oferty dla klientow/001 Spis ofert.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2aace290947994e4/000 B^0R Projekt/000 Dokumenty Ogolne/04 Oferty dla klientow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_9248486D44C93C52631DEA188F3E8C1851038387" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36780057-F997-4C2C-8758-1232FB34E9BF}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_9248486D44C93C52631DEA188F3E8C1851038387" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8672D624-C64B-4CED-ABAA-6CD8D1FEB197}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Nr Oferty</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>Nr porzadkowy</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>13.07.2022</t>
+  </si>
+  <si>
+    <t>12.08.2022</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>C\.....</t>
   </si>
 </sst>
 </file>
@@ -581,7 +596,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Arkusz1"/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -630,13 +645,50 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="6">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>